<commit_message>
2 bancos de dados finalizados
</commit_message>
<xml_diff>
--- a/resultados_ajuste_a_dados_reais.xlsx
+++ b/resultados_ajuste_a_dados_reais.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NetoDavi\Desktop\survival_pibic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BDA699-DDB2-412A-999D-0BE00900F015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81D5DAC-0EAB-4891-A7BF-350F08D0AD45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{6BDB12EF-AC99-404F-A874-0220E9463E94}"/>
   </bookViews>
   <sheets>
-    <sheet name="smoke_cessation_Bannerger2009" sheetId="1" r:id="rId1"/>
-    <sheet name="aneurysm" sheetId="2" r:id="rId2"/>
+    <sheet name="breast_cancer" sheetId="6" r:id="rId1"/>
+    <sheet name="smoke_cessation_Bannerger2009" sheetId="1" r:id="rId2"/>
+    <sheet name="hemo.icens" sheetId="5" r:id="rId3"/>
+    <sheet name="aneurysm" sheetId="2" r:id="rId4"/>
+    <sheet name="aidscohort.y" sheetId="3" r:id="rId5"/>
+    <sheet name="aidscohort.z" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="8">
   <si>
     <t>AIC</t>
   </si>
@@ -66,8 +70,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="169" formatCode="#,##0.000"/>
-    <numFmt numFmtId="170" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -98,13 +102,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,11 +423,425 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ABE0690-CB0A-4D62-BB83-602469341B46}">
-  <dimension ref="C2:U8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4D33930-F2E1-4177-9C6E-D1890C899ABE}">
+  <dimension ref="B2:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:E4"/>
+      <selection activeCell="I21" sqref="I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="31.7109375" customWidth="1"/>
+    <col min="14" max="14" width="40.28515625" customWidth="1"/>
+    <col min="18" max="18" width="15.28515625" customWidth="1"/>
+    <col min="19" max="19" width="19.42578125" customWidth="1"/>
+    <col min="20" max="20" width="27.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>292.06610000000001</v>
+      </c>
+      <c r="C4" s="1">
+        <v>372.38869999999997</v>
+      </c>
+      <c r="D4" s="1">
+        <v>343.5849</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>304.06183136645399</v>
+      </c>
+      <c r="H4" s="1">
+        <v>316.77830527780401</v>
+      </c>
+      <c r="I4" s="1">
+        <v>309.19835608455998</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5" s="1">
+        <v>298.35023608316601</v>
+      </c>
+      <c r="H5" s="1">
+        <v>313.61000477678601</v>
+      </c>
+      <c r="I5" s="1">
+        <v>304.51406574489403</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C6" s="4"/>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6" s="1">
+        <v>299.889557326621</v>
+      </c>
+      <c r="H6" s="1">
+        <v>317.69262080251099</v>
+      </c>
+      <c r="I6" s="1">
+        <v>307.08069193197002</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7" s="1">
+        <v>299.79116741165501</v>
+      </c>
+      <c r="H7" s="1">
+        <v>320.13752566981498</v>
+      </c>
+      <c r="I7" s="1">
+        <v>308.009606960626</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8" s="1">
+        <v>301.208207461406</v>
+      </c>
+      <c r="H8" s="1">
+        <v>324.09786050183601</v>
+      </c>
+      <c r="I8" s="1">
+        <v>310.453951953998</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>7</v>
+      </c>
+      <c r="G9" s="1">
+        <v>304.45128178218499</v>
+      </c>
+      <c r="H9" s="1">
+        <v>329.88422960488498</v>
+      </c>
+      <c r="I9" s="1">
+        <v>314.72433121839703</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10" s="1">
+        <v>305.46033161769901</v>
+      </c>
+      <c r="H10" s="1">
+        <v>333.43657422266898</v>
+      </c>
+      <c r="I10" s="1">
+        <v>316.76068599753302</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1">
+        <v>294.056919813587</v>
+      </c>
+      <c r="H14" s="1">
+        <v>304.23009894266698</v>
+      </c>
+      <c r="I14" s="1">
+        <v>298.16613958807199</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="G15" s="1">
+        <v>295.50399625248099</v>
+      </c>
+      <c r="H15" s="1">
+        <v>308.22047016383101</v>
+      </c>
+      <c r="I15" s="1">
+        <v>300.64052097058698</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>4</v>
+      </c>
+      <c r="G16" s="1">
+        <v>296.873821500698</v>
+      </c>
+      <c r="H16" s="1">
+        <v>312.133590194318</v>
+      </c>
+      <c r="I16" s="1">
+        <v>303.03765116242602</v>
+      </c>
+    </row>
+    <row r="17" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>5</v>
+      </c>
+      <c r="G17" s="1">
+        <v>298.44125170835099</v>
+      </c>
+      <c r="H17" s="1">
+        <v>316.24431518424097</v>
+      </c>
+      <c r="I17" s="1">
+        <v>305.63238631370001</v>
+      </c>
+    </row>
+    <row r="18" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>6</v>
+      </c>
+      <c r="G18" s="1">
+        <v>299.25719541508403</v>
+      </c>
+      <c r="H18" s="1">
+        <v>319.60355367324399</v>
+      </c>
+      <c r="I18" s="1">
+        <v>307.475634964054</v>
+      </c>
+    </row>
+    <row r="19" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>7</v>
+      </c>
+      <c r="G19" s="1">
+        <v>300.89450683218001</v>
+      </c>
+      <c r="H19" s="1">
+        <v>323.78415987261002</v>
+      </c>
+      <c r="I19" s="1">
+        <v>310.14025132477201</v>
+      </c>
+    </row>
+    <row r="20" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>8</v>
+      </c>
+      <c r="G20" s="1">
+        <v>302.53658621230102</v>
+      </c>
+      <c r="H20" s="1">
+        <v>327.969534035001</v>
+      </c>
+      <c r="I20" s="1">
+        <v>312.80963564851299</v>
+      </c>
+    </row>
+    <row r="25" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="G25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" t="s">
+        <v>0</v>
+      </c>
+      <c r="H26" t="s">
+        <v>1</v>
+      </c>
+      <c r="I26" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27" s="1">
+        <v>297.04319894224301</v>
+      </c>
+      <c r="H27" s="1">
+        <v>312.30296763586301</v>
+      </c>
+      <c r="I27" s="1">
+        <v>303.20702860397103</v>
+      </c>
+    </row>
+    <row r="28" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>3</v>
+      </c>
+      <c r="G28" s="1">
+        <v>297.57643640723199</v>
+      </c>
+      <c r="H28" s="1">
+        <v>315.37949988312198</v>
+      </c>
+      <c r="I28" s="1">
+        <v>304.76757101258102</v>
+      </c>
+    </row>
+    <row r="29" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>4</v>
+      </c>
+      <c r="G29" s="1">
+        <v>298.91166083861498</v>
+      </c>
+      <c r="H29" s="1">
+        <v>319.258019096775</v>
+      </c>
+      <c r="I29" s="1">
+        <v>307.130100387585</v>
+      </c>
+    </row>
+    <row r="30" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>5</v>
+      </c>
+      <c r="G30" s="1">
+        <v>300.12153194757701</v>
+      </c>
+      <c r="H30" s="1">
+        <v>323.01118498800702</v>
+      </c>
+      <c r="I30" s="1">
+        <v>309.36727644016798</v>
+      </c>
+    </row>
+    <row r="31" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>6</v>
+      </c>
+      <c r="G31" s="1">
+        <v>300.97852494442498</v>
+      </c>
+      <c r="H31" s="1">
+        <v>326.41147276712502</v>
+      </c>
+      <c r="I31" s="1">
+        <v>311.25157438063798</v>
+      </c>
+    </row>
+    <row r="32" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <v>7</v>
+      </c>
+      <c r="G32" s="1">
+        <v>303.08077374825302</v>
+      </c>
+      <c r="H32" s="1">
+        <v>331.05701635322299</v>
+      </c>
+      <c r="I32" s="1">
+        <v>314.38112812808703</v>
+      </c>
+    </row>
+    <row r="33" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>8</v>
+      </c>
+      <c r="G33" s="1">
+        <v>304.43458069178098</v>
+      </c>
+      <c r="H33" s="1">
+        <v>334.95411807902099</v>
+      </c>
+      <c r="I33" s="1">
+        <v>316.76224001523599</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="G25:I25"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ABE0690-CB0A-4D62-BB83-602469341B46}">
+  <dimension ref="C2:J29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,192 +859,220 @@
     <col min="21" max="21" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="H2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="M2" s="1" t="s">
+    <row r="2" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="H2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C4" s="2">
+        <v>431.41250000000002</v>
+      </c>
+      <c r="D4" s="2">
+        <v>451.85559999999998</v>
+      </c>
+      <c r="E4" s="2">
+        <v>439.6653</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4" s="2">
+        <v>441.56220000000002</v>
+      </c>
+      <c r="I4" s="2">
+        <v>479.04109999999997</v>
+      </c>
+      <c r="J4" s="2">
+        <v>456.69220000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5" s="2">
+        <v>443.52519999999998</v>
+      </c>
+      <c r="I5" s="2">
+        <v>484.41129999999998</v>
+      </c>
+      <c r="J5" s="2">
+        <v>460.03059999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="G7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="H12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="S2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-    </row>
-    <row r="3" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L3" t="s">
-        <v>4</v>
-      </c>
-      <c r="M3" t="s">
-        <v>0</v>
-      </c>
-      <c r="N3" t="s">
-        <v>1</v>
-      </c>
-      <c r="O3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R3" t="s">
-        <v>4</v>
-      </c>
-      <c r="S3" t="s">
-        <v>0</v>
-      </c>
-      <c r="T3" t="s">
-        <v>1</v>
-      </c>
-      <c r="U3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C4" s="3">
-        <v>431.41250000000002</v>
-      </c>
-      <c r="D4" s="3">
-        <v>451.85559999999998</v>
-      </c>
-      <c r="E4" s="3">
-        <v>439.6653</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-      <c r="H4" s="3">
-        <v>441.56220000000002</v>
-      </c>
-      <c r="I4" s="3">
-        <v>479.04109999999997</v>
-      </c>
-      <c r="J4" s="3">
-        <v>456.69220000000001</v>
-      </c>
-      <c r="L4">
-        <v>2</v>
-      </c>
-      <c r="M4" s="3">
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" t="s">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14" s="2">
         <v>427.62200000000001</v>
       </c>
-      <c r="N4" s="3">
+      <c r="I14" s="2">
         <v>451.47219999999999</v>
       </c>
-      <c r="O4" s="3">
+      <c r="J14" s="2">
         <v>437.25020000000001</v>
       </c>
-      <c r="R4">
-        <v>2</v>
-      </c>
-      <c r="S4" s="2">
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>3</v>
+      </c>
+      <c r="H15" s="2">
+        <v>395.2303</v>
+      </c>
+      <c r="I15" s="2">
+        <v>422.48759999999999</v>
+      </c>
+      <c r="J15" s="2">
+        <v>406.23390000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="H23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" t="s">
+        <v>0</v>
+      </c>
+      <c r="I24" t="s">
+        <v>1</v>
+      </c>
+      <c r="J24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25" s="1">
         <v>405.44990000000001</v>
       </c>
-      <c r="T4" s="2">
+      <c r="I25" s="1">
         <v>446.33600000000001</v>
       </c>
-      <c r="U4" s="2">
+      <c r="J25" s="1">
         <v>421.9554</v>
       </c>
     </row>
-    <row r="5" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="G5">
-        <v>3</v>
-      </c>
-      <c r="H5" s="3">
-        <v>443.52519999999998</v>
-      </c>
-      <c r="I5" s="3">
-        <v>484.41129999999998</v>
-      </c>
-      <c r="J5" s="3">
-        <v>460.03059999999999</v>
-      </c>
-      <c r="L5">
-        <v>3</v>
-      </c>
-      <c r="M5" s="3">
-        <v>395.2303</v>
-      </c>
-      <c r="N5" s="3">
-        <v>422.48759999999999</v>
-      </c>
-      <c r="O5" s="3">
-        <v>406.23390000000001</v>
-      </c>
-      <c r="R5">
-        <v>3</v>
-      </c>
-      <c r="S5" s="2">
+    <row r="26" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <v>3</v>
+      </c>
+      <c r="H26" s="1">
         <v>391.10340000000002</v>
       </c>
-      <c r="T5" s="2">
+      <c r="I26" s="1">
         <v>435.39659999999998</v>
       </c>
-      <c r="U5" s="2">
+      <c r="J26" s="1">
         <v>408.98430000000002</v>
       </c>
     </row>
-    <row r="6" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="G6">
-        <v>4</v>
-      </c>
-      <c r="L6">
-        <v>4</v>
-      </c>
-      <c r="R6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="G7">
-        <v>5</v>
-      </c>
-      <c r="L7">
-        <v>5</v>
-      </c>
-      <c r="R7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="G8">
-        <v>6</v>
-      </c>
-      <c r="L8">
-        <v>6</v>
-      </c>
-      <c r="R8">
+    <row r="27" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G29">
         <v>6</v>
       </c>
     </row>
@@ -633,19 +1080,194 @@
   <mergeCells count="4">
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="H2:J2"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="H23:J23"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F289A84B-9A34-4444-8EB5-BAD8E4DA2F77}">
+  <dimension ref="B2:T8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="31.7109375" customWidth="1"/>
+    <col min="14" max="14" width="40.28515625" customWidth="1"/>
+    <col min="18" max="18" width="15.28515625" customWidth="1"/>
+    <col min="19" max="19" width="19.42578125" customWidth="1"/>
+    <col min="20" max="20" width="27.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="L2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="R2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>4</v>
+      </c>
+      <c r="R3" t="s">
+        <v>0</v>
+      </c>
+      <c r="S3" t="s">
+        <v>1</v>
+      </c>
+      <c r="T3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="Q4">
+        <v>2</v>
+      </c>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="Q5">
+        <v>3</v>
+      </c>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="Q6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="K7">
+        <v>5</v>
+      </c>
+      <c r="Q7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="K8">
+        <v>6</v>
+      </c>
+      <c r="Q8">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="R2:T2"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{526A8161-0B58-4A43-B384-C59D4BEB848E}">
   <dimension ref="C2:U8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5:N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,26 +1286,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="H2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="M2" s="1" t="s">
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="H2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="M2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="S2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="S2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
     </row>
     <row r="3" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
@@ -733,37 +1355,37 @@
       </c>
     </row>
     <row r="4" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>189.30840000000001</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>204.32810000000001</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>195.41069999999999</v>
       </c>
       <c r="G4">
         <v>2</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
       <c r="L4">
         <v>2</v>
       </c>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
       <c r="R4">
         <v>2</v>
       </c>
-      <c r="S4" s="3">
+      <c r="S4" s="2">
         <v>196.55179999999999</v>
       </c>
-      <c r="T4" s="3">
+      <c r="T4" s="2">
         <v>226.59129999999999</v>
       </c>
-      <c r="U4" s="3">
+      <c r="U4" s="2">
         <v>208.75640000000001</v>
       </c>
     </row>
@@ -771,31 +1393,31 @@
       <c r="G5">
         <v>3</v>
       </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
       <c r="L5">
         <v>3</v>
       </c>
-      <c r="M5" s="3">
+      <c r="M5" s="2">
         <v>191.74520000000001</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5" s="2">
         <v>212.77289999999999</v>
       </c>
-      <c r="O5" s="3">
+      <c r="O5" s="2">
         <v>200.2884</v>
       </c>
       <c r="R5">
         <v>3</v>
       </c>
-      <c r="S5" s="3">
+      <c r="S5" s="2">
         <v>197.14660000000001</v>
       </c>
-      <c r="T5" s="3">
+      <c r="T5" s="2">
         <v>230.19</v>
       </c>
-      <c r="U5" s="3">
+      <c r="U5" s="2">
         <v>210.57149999999999</v>
       </c>
     </row>
@@ -811,8 +1433,8 @@
       </c>
     </row>
     <row r="7" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
       <c r="G7">
         <v>5</v>
       </c>
@@ -843,4 +1465,483 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA5A1B81-A0EE-47D9-9387-77A3E5FDAC1B}">
+  <dimension ref="B3:T10"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" customWidth="1"/>
+    <col min="13" max="13" width="21.85546875" customWidth="1"/>
+    <col min="14" max="14" width="22" customWidth="1"/>
+    <col min="18" max="18" width="21.5703125" customWidth="1"/>
+    <col min="19" max="19" width="16.28515625" customWidth="1"/>
+    <col min="20" max="20" width="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="G3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="L3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="R3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>4</v>
+      </c>
+      <c r="R4" t="s">
+        <v>0</v>
+      </c>
+      <c r="S4" t="s">
+        <v>1</v>
+      </c>
+      <c r="T4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <v>794.82839999999999</v>
+      </c>
+      <c r="C5" s="2">
+        <v>809.02470000000005</v>
+      </c>
+      <c r="D5" s="2">
+        <v>800.53750000000002</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="Q5">
+        <v>2</v>
+      </c>
+      <c r="R5" s="2">
+        <v>835.18140000000005</v>
+      </c>
+      <c r="S5" s="2">
+        <v>863.57399999999996</v>
+      </c>
+      <c r="T5" s="2">
+        <v>846.59950000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="Q6">
+        <v>3</v>
+      </c>
+      <c r="R6" s="2">
+        <v>837127</v>
+      </c>
+      <c r="S6" s="2">
+        <v>8690687</v>
+      </c>
+      <c r="T6" s="2">
+        <v>8499724</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="K7">
+        <v>4</v>
+      </c>
+      <c r="Q7">
+        <v>4</v>
+      </c>
+      <c r="R7" s="2">
+        <v>838.04049999999995</v>
+      </c>
+      <c r="S7" s="2">
+        <v>8735313</v>
+      </c>
+      <c r="T7" s="2">
+        <v>8523132</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <v>5</v>
+      </c>
+      <c r="Q8">
+        <v>5</v>
+      </c>
+      <c r="R8" s="2">
+        <v>811.95709999999997</v>
+      </c>
+      <c r="S8" s="2">
+        <v>8509969</v>
+      </c>
+      <c r="T8" s="2">
+        <v>827657</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="K9">
+        <v>6</v>
+      </c>
+      <c r="Q9">
+        <v>7</v>
+      </c>
+      <c r="R9" s="2">
+        <v>822.14</v>
+      </c>
+      <c r="S9" s="2">
+        <v>868278</v>
+      </c>
+      <c r="T9" s="2">
+        <v>8406944</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="Q10">
+        <v>10</v>
+      </c>
+      <c r="R10" s="2">
+        <v>805.97289999999998</v>
+      </c>
+      <c r="S10" s="2">
+        <v>8627582</v>
+      </c>
+      <c r="T10" s="2">
+        <v>8288092</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="R3:T3"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A03AE184-D6A5-4907-9497-2796EC9B3B67}">
+  <dimension ref="B2:T9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" customWidth="1"/>
+    <col min="13" max="13" width="19" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" customWidth="1"/>
+    <col min="18" max="18" width="17.140625" customWidth="1"/>
+    <col min="19" max="19" width="15.28515625" customWidth="1"/>
+    <col min="20" max="20" width="22.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="L2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="R2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>4</v>
+      </c>
+      <c r="R3" t="s">
+        <v>0</v>
+      </c>
+      <c r="S3" t="s">
+        <v>1</v>
+      </c>
+      <c r="T3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
+        <v>412.12029999999999</v>
+      </c>
+      <c r="C4" s="2">
+        <v>426.31659999999999</v>
+      </c>
+      <c r="D4" s="2">
+        <v>417.82929999999999</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="Q4">
+        <v>2</v>
+      </c>
+      <c r="R4" s="2">
+        <v>994.6223</v>
+      </c>
+      <c r="S4" s="2">
+        <v>1023.015</v>
+      </c>
+      <c r="T4" s="2">
+        <v>1006.04</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="Q5">
+        <v>3</v>
+      </c>
+      <c r="R5" s="2">
+        <v>995.34630000000004</v>
+      </c>
+      <c r="S5" s="2">
+        <v>1027.288</v>
+      </c>
+      <c r="T5" s="2">
+        <v>1008.192</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="Q6">
+        <v>5</v>
+      </c>
+      <c r="R6" s="2">
+        <v>998.44979999999998</v>
+      </c>
+      <c r="S6" s="2">
+        <v>1037.49</v>
+      </c>
+      <c r="T6" s="2">
+        <v>1014.15</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="K7">
+        <v>5</v>
+      </c>
+      <c r="Q7">
+        <v>7</v>
+      </c>
+      <c r="R7" s="2">
+        <v>996.6848</v>
+      </c>
+      <c r="S7" s="2">
+        <v>1042.8230000000001</v>
+      </c>
+      <c r="T7" s="2">
+        <v>1015.239</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="K8">
+        <v>6</v>
+      </c>
+      <c r="Q8">
+        <v>9</v>
+      </c>
+      <c r="R8" s="2">
+        <v>1003.735</v>
+      </c>
+      <c r="S8" s="2">
+        <v>1056.972</v>
+      </c>
+      <c r="T8" s="2">
+        <v>1025.144</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="Q9">
+        <v>10</v>
+      </c>
+      <c r="R9" s="2">
+        <v>997.56050000000005</v>
+      </c>
+      <c r="S9" s="2">
+        <v>1054.346</v>
+      </c>
+      <c r="T9" s="2">
+        <v>1020.397</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="R2:T2"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
repaginacao MC e dados para teste
</commit_message>
<xml_diff>
--- a/resultados_ajuste_a_dados_reais.xlsx
+++ b/resultados_ajuste_a_dados_reais.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NetoDavi\Desktop\survival_pibic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81D5DAC-0EAB-4891-A7BF-350F08D0AD45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6128CC-87D8-487F-A2D7-22F8837DBCB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{6BDB12EF-AC99-404F-A874-0220E9463E94}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="15">
   <si>
     <t>AIC</t>
   </si>
@@ -63,6 +63,27 @@
   </si>
   <si>
     <t>Modelo Exponencial por partes potencia sem fracao de cura</t>
+  </si>
+  <si>
+    <t>Estimativas</t>
+  </si>
+  <si>
+    <t>chute = c(c(2,0.3,70,75),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          1.2,0.1,0.1,0.1,0.1,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.1,0.1,0.1,0.1)</t>
+  </si>
+  <si>
+    <t>chute = c(c(2,0.3,70),</t>
+  </si>
+  <si>
+    <t>chute = c(c(2,0.3,20,65,120),</t>
+  </si>
+  <si>
+    <t>chute = c(c(5,3,2,65,100,300),</t>
   </si>
 </sst>
 </file>
@@ -106,10 +127,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,12 +447,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4D33930-F2E1-4177-9C6E-D1890C899ABE}">
   <dimension ref="B2:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
     <col min="7" max="7" width="17.5703125" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
     <col min="9" max="9" width="31.7109375" customWidth="1"/>
@@ -442,16 +464,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="G2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="G2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -481,10 +503,10 @@
         <v>292.06610000000001</v>
       </c>
       <c r="C4" s="1">
-        <v>372.38869999999997</v>
+        <v>299.69600000000003</v>
       </c>
       <c r="D4" s="1">
-        <v>343.5849</v>
+        <v>295.14800000000002</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -514,7 +536,7 @@
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C6" s="4"/>
+      <c r="C6" s="3"/>
       <c r="F6">
         <v>4</v>
       </c>
@@ -588,11 +610,11 @@
     </row>
     <row r="11" spans="2:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
@@ -707,11 +729,11 @@
       </c>
     </row>
     <row r="25" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="G25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
+      <c r="G25" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
     </row>
     <row r="26" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F26" t="s">
@@ -838,10 +860,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ABE0690-CB0A-4D62-BB83-602469341B46}">
-  <dimension ref="C2:J29"/>
+  <dimension ref="C2:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24:Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,25 +873,28 @@
     <col min="8" max="8" width="15.7109375" customWidth="1"/>
     <col min="9" max="9" width="21.85546875" customWidth="1"/>
     <col min="10" max="10" width="18" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18.85546875" customWidth="1"/>
-    <col min="14" max="14" width="16.5703125" customWidth="1"/>
-    <col min="15" max="15" width="21" customWidth="1"/>
+    <col min="14" max="14" width="22" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.28515625" customWidth="1"/>
+    <col min="16" max="16" width="26.7109375" customWidth="1"/>
+    <col min="17" max="17" width="25.85546875" customWidth="1"/>
     <col min="19" max="19" width="14.42578125" customWidth="1"/>
     <col min="20" max="20" width="19" customWidth="1"/>
     <col min="21" max="21" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="H2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="H2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
     </row>
     <row r="3" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
@@ -949,11 +974,11 @@
       </c>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.25">
       <c r="G13" t="s">
@@ -1002,24 +1027,36 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G17">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G18">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="H23" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-    </row>
-    <row r="24" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="H23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="N23">
+        <v>3</v>
+      </c>
+      <c r="O23">
+        <v>4</v>
+      </c>
+      <c r="P23">
+        <v>5</v>
+      </c>
+      <c r="Q23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G24" t="s">
         <v>4</v>
       </c>
@@ -1032,48 +1069,136 @@
       <c r="J24" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="L24" t="s">
+        <v>8</v>
+      </c>
+      <c r="N24" t="s">
+        <v>12</v>
+      </c>
+      <c r="O24" t="s">
+        <v>9</v>
+      </c>
+      <c r="P24" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G25">
         <v>2</v>
       </c>
       <c r="H25" s="1">
-        <v>405.44990000000001</v>
+        <v>395.37020000000001</v>
       </c>
       <c r="I25" s="1">
-        <v>446.33600000000001</v>
+        <v>436.25619999999998</v>
       </c>
       <c r="J25" s="1">
-        <v>421.9554</v>
-      </c>
-    </row>
-    <row r="26" spans="7:10" x14ac:dyDescent="0.25">
+        <v>411.87560000000002</v>
+      </c>
+      <c r="N25">
+        <v>10</v>
+      </c>
+      <c r="O25">
+        <v>10</v>
+      </c>
+      <c r="P25">
+        <v>200</v>
+      </c>
+      <c r="Q25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G26">
         <v>3</v>
       </c>
       <c r="H26" s="1">
-        <v>391.10340000000002</v>
+        <v>391.51749999999998</v>
       </c>
       <c r="I26" s="1">
-        <v>435.39659999999998</v>
+        <v>435.81079999999997</v>
       </c>
       <c r="J26" s="1">
-        <v>408.98430000000002</v>
-      </c>
-    </row>
-    <row r="27" spans="7:10" x14ac:dyDescent="0.25">
+        <v>409.39839999999998</v>
+      </c>
+      <c r="N26" t="s">
+        <v>10</v>
+      </c>
+      <c r="O26" t="s">
+        <v>10</v>
+      </c>
+      <c r="P26" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G27">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="H27" s="1">
+        <v>400.30160000000001</v>
+      </c>
+      <c r="I27" s="1">
+        <v>448.00200000000001</v>
+      </c>
+      <c r="J27" s="1">
+        <v>419.55790000000002</v>
+      </c>
+      <c r="N27" t="s">
+        <v>11</v>
+      </c>
+      <c r="O27" t="s">
+        <v>11</v>
+      </c>
+      <c r="P27" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G28">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="H28" s="1">
+        <v>403.46289999999999</v>
+      </c>
+      <c r="I28" s="1">
+        <v>454.57049999999998</v>
+      </c>
+      <c r="J28" s="1">
+        <v>424.09469999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G29">
         <v>6</v>
+      </c>
+      <c r="H29" s="1">
+        <v>371.30779999999999</v>
+      </c>
+      <c r="I29" s="1">
+        <v>425.82260000000002</v>
+      </c>
+      <c r="J29" s="1">
+        <v>393.31509999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G30">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1105,26 +1230,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="G2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="L2" s="3" t="s">
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="G2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="L2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="R2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="R2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -1286,26 +1411,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="H2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="M2" s="3" t="s">
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="H2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="M2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="S2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="S2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
     </row>
     <row r="3" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
@@ -1489,26 +1614,26 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="G3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="L3" s="3" t="s">
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="G3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="L3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="R3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="R3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -1730,26 +1855,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="G2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="L2" s="3" t="s">
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="G2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="L2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="R2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="R2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B3" t="s">

</xml_diff>